<commit_message>
save 14 11 2025
</commit_message>
<xml_diff>
--- a/4 четверть_13_JavaScript_sugarJS.xlsx
+++ b/4 четверть_13_JavaScript_sugarJS.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3929DF-58BF-4C9E-B634-7735120DE2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C17255-BEC7-4749-8D83-B9170DADDE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sugarjs" sheetId="20" r:id="rId1"/>
     <sheet name="Array" sheetId="15" r:id="rId2"/>
     <sheet name="Date" sheetId="18" r:id="rId3"/>
     <sheet name="Object" sheetId="19" r:id="rId4"/>
+    <sheet name="String" sheetId="21" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="827">
   <si>
     <t>construct(n,indexMapFn)</t>
   </si>
@@ -10923,6 +10924,2114 @@
         <scheme val="minor"/>
       </rPr>
       <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>at(index,[loop] = false)</t>
+  </si>
+  <si>
+    <t>Gets the character(s) at a given index. When loop is true, overshooting the end of the string will begin counting from the other end. index may be negative. If index is an array, multiple elements will be returned.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">select </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String</t>
+    </r>
+  </si>
+  <si>
+    <t>camelize([upper] = true)</t>
+  </si>
+  <si>
+    <t>Converts underscores and hyphens to camel case. If upper is true, the string will be UpperCamelCase. If the inflections module is included, acronyms can also be defined that will be used when camelizing.</t>
+  </si>
+  <si>
+    <t>'caps_lock'.camelize() //"CapsLock"
+'moz-border-radius'.camelize() //"MozBorderRadius"
+'moz-border-radius'.camelize(false) //"mozBorderRadius"
+'http-method'.camelize() //"HTTPMethod"</t>
+  </si>
+  <si>
+    <t>capitalize([lower] = false,[all] = false)</t>
+  </si>
+  <si>
+    <t>Capitalizes the first character of the string. If lower is true, the remainder of the string will be downcased. If all is true, all words in the string will be capitalized.</t>
+  </si>
+  <si>
+    <t>chars(eachCharFn)</t>
+  </si>
+  <si>
+    <t>Runs eachCharFn against each character in the string, and returns an array.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jumpy'.chars()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> //["j", "u", "m", "p", "y"]
+'jumpy'.chars(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function(c) {
+  // Called 5 times: "j","u","m","p","y"
+}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">); //["j", "u", "m", "p", "y"]
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>hello'.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>capitalize()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> //"Hello"
+'HELLO'.capitalize(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //"Hello"
+'hello kitty'.capitalize() //"Hello kitty"
+'hEllO kItTy'.capitalize(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>true, true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //"Hello Kitty"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>'jumpy'.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>at(0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> //"j"
+'jumpy'.at(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //"y"
+'jumpy'.at(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //""
+'jumpy'.at(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5, true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //"j"
+'lucky charms'.at(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2, 4]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) //["c", "y"]
+</t>
+    </r>
+  </si>
+  <si>
+    <t>modify String</t>
+  </si>
+  <si>
+    <t>codes([eachCodeFn])</t>
+  </si>
+  <si>
+    <r>
+      <t>jumpy'.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">codes() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//[106, 117, 109, 112, 121]
+'jumpy'.codes(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function(c) {
+  // Called 5 times: 106, 117, 109, 112, 121
+}); //[106, 117, 109, 112, 121]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">get </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Array</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>of Codes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">get </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Array of Chars</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">modify </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String</t>
+    </r>
+  </si>
+  <si>
+    <t>Runs callback eachCodeFn against each character code in the string. Returns an array of character codes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+code	The current character code.
+i	The current index.
+str	The string being operated on.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+char	The current character.
+i	The current index.
+arr	An array of all characters.</t>
+  </si>
+  <si>
+    <t>compact()</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>too \n much \n space'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.compact() //"too much space"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'enough \n '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.compact() //"enough"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Compacts </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>whitespace (пробелы и переносы строки)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the string to a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>single space</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>trims</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the ends.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>trim()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>string.replace(' \n ', ' ')</t>
+    </r>
+  </si>
+  <si>
+    <t>dasherize()</t>
+  </si>
+  <si>
+    <t>a_farewell_to_arms'.dasherize() //"a-farewell-to-arms"
+'capsLock'.dasherize() //"caps-lock"</t>
+  </si>
+  <si>
+    <t>Converts underscores and camel casing to hypens.</t>
+  </si>
+  <si>
+    <t>decodeBase64()</t>
+  </si>
+  <si>
+    <t>Decodes the string from base64 encoding. This method wraps native methods when available, and uses a custom implementation when not available. It can also handle Unicode string encodings.</t>
+  </si>
+  <si>
+    <r>
+      <t>aHR0cDovL3R3aXR0ZXIuY29tLw=='.decodeBase64() //</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"http://twitter.com/"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+'anVzdCBnb3QgZGVjb2RlZA=='.decodeBase64() //</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"just got decoded"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Decode </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>coding</t>
+    </r>
+  </si>
+  <si>
+    <t>encodeBase64()</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">gonna get encoded!'.encodeBase64() </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//"Z29ubmEgZ2V0IGVuY29kZWQh"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+'http://twitter.com/'.encodeBase64() </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//"aHR0cDovL3R3aXR0ZXIuY29tLw=="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Encodes the string into base64 encoding. This method wraps native methods when available, and uses a custom implementation when not available. It can also handle Unicode string encodings.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Encode </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> into </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>coding</t>
+    </r>
+  </si>
+  <si>
+    <t>endsWith(search,[pos] = length)</t>
+  </si>
+  <si>
+    <t>Returns true if the string ends with substring search. Search ends at pos, which defaults to the entire string length. This method is provided as a polyfill.</t>
+  </si>
+  <si>
+    <r>
+      <t>jum</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'.endsWith('</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>') //true
+'ju</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mpy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'.endsWith('</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MPY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>')  //false
+'ju</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>y'.endsWith(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'mp', 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)  //true</t>
+    </r>
+  </si>
+  <si>
+    <t>first([n] = 1)</t>
+  </si>
+  <si>
+    <t>Returns the first n characters of the string.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ucky charms'.first() //"l"
+'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>luc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ky charms'.first(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //"luc"</t>
+    </r>
+  </si>
+  <si>
+    <t>forEach([search],[eachFn])</t>
+  </si>
+  <si>
+    <t>Runs callback eachFn against every character in the string, or every every occurence of search if it is provided. Returns an array of matches. search may be either a string or regex, and defaults to every character in the string. If eachFn returns false at any time it will break out of the loop.</t>
+  </si>
+  <si>
+    <t>match	The current match.
+i	The current index.
+arr	An array of all matches.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">jumpy'.forEach(console.log)
+'jumpy'.forEach(log) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//["j", "u", "m", "p", "y"]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>неуверен</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+'jumpy'.forEach(/[r-z]/) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>["u", "y"]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+'jumpy'.forEach(/mp/)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ["mp"]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+'jumpy'.forEach(/[r-z]/, function(m) {
+  // Called twice: "u", "y"
+}); //["u", "y"]</t>
+    </r>
+  </si>
+  <si>
+    <t>format(obj1,[obj2],[...)</t>
+  </si>
+  <si>
+    <t>Replaces {} tokens in the string with arguments or properties. Tokens support deep properties. If a single object is passed, its properties can be accessed by keywords such as {name}. If multiple objects or a non-object are passed, they can be accessed by the argument position like {0}. Literal braces in the string can be escaped by repeating them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome, {name}.'.format({ name: 'Bill' })
+'You are {0} years old today.'.format(5)
+'{0.name} and {1.name}'.format(users)
+'${currencies.usd.balance}'.format(Harry) //"$482"
+'{{Hello}}'.format('Hello') //"{Hello}"
+</t>
+  </si>
+  <si>
+    <t>Форматированная строка</t>
+  </si>
+  <si>
+    <t>from([index] = 0)</t>
+  </si>
+  <si>
+    <t>Returns a section of the string starting from index.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">'lucky charms'.from() </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//"lucky charms"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+'lucky charms'.from(7) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//"harms"</t>
+    </r>
+  </si>
+  <si>
+    <t>hasScript()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>Returns true if the string contains any characters in that script.
+hasArabic
+hasCyrillic
+hasGreek
+hasHangul
+hasHan
+hasKanji
+hasHebrew
+hasHiragana
+hasKana
+hasKatakana
+hasLatin
+hasThai
+hasDevanagari</t>
+  </si>
+  <si>
+    <t>includes</t>
+  </si>
+  <si>
+    <t>'jumpy'.includes('py') //true
+'broken'.includes('ken', 3) //true
+'broken'.includes('bro', 3) //false</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Returns true if search is contained within the string. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Search begins at pos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, which defaults to the beginning of the string. 
+Sugar enhances this method to allow matching a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>regex</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+This method is provided as a polyfill.</t>
+    </r>
+  </si>
+  <si>
+    <t>Boolean
++regex</t>
+  </si>
+  <si>
+    <t>insert(str,[index] = length)</t>
+  </si>
+  <si>
+    <t>Adds str at index. Allows negative values.</t>
+  </si>
+  <si>
+    <t>'dopamine'.insert('e', 3) //"dopeamine"
+'spelling eror'.insert('r', -3) //"spelling error"</t>
+  </si>
+  <si>
+    <t>isBlank()</t>
+  </si>
+  <si>
+    <t>'.isBlank() //true
+'   '.isBlank() //true
+'noway'.isBlank() //false</t>
+  </si>
+  <si>
+    <t>''.isEmpty() //true
+' '.isEmpty() //false
+'a'.isEmpty() //false</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Returns true if the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>string has length 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Returns true if the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>string has length 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> contains only whitespace.</t>
+    </r>
+  </si>
+  <si>
+    <t>last([n] = 1)</t>
+  </si>
+  <si>
+    <t>Returns the last n characters of the string.</t>
+  </si>
+  <si>
+    <r>
+      <t>lucky charm</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'.last() //"s"
+'lucky cha</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'.last(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //"rms"</t>
+    </r>
+  </si>
+  <si>
+    <t>Runs eachLineFn against each line in the string, and returns an array.</t>
+  </si>
+  <si>
+    <r>
+      <t>lineText.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">lines() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//["Line one.", "Line two.", "Line three."]
+lineText.lines(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function(l) {
+  // Called once per line
+});</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> //["Line one.", "Line two.", "Line three."]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">get </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Array of Lines</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String</t>
+    </r>
+  </si>
+  <si>
+    <t>lines([eachLineFn])</t>
+  </si>
+  <si>
+    <t>pad(num,[padding] = ' ')</t>
+  </si>
+  <si>
+    <t>Pads the string out with padding to be exactly num characters.</t>
+  </si>
+  <si>
+    <r>
+      <t>'wasabi'.pad(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //" wasabi "
+'wasabi'.pad(8,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> '-'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //"-wasabi-"</t>
+    </r>
+  </si>
+  <si>
+    <t>padLeft(num,padding)</t>
+  </si>
+  <si>
+    <t>Pads the string out from the left with padding to be exactly num characters.</t>
+  </si>
+  <si>
+    <r>
+      <t>'wasabi'.padLeft(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //" wasabi"
+'wasabi'.padLeft(8,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> '-'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //"--wasabi"</t>
+    </r>
+  </si>
+  <si>
+    <t>padRight(num,[padding] = ' ')</t>
+  </si>
+  <si>
+    <t>Pads the string out from the right with padding to be exactly num characters.</t>
+  </si>
+  <si>
+    <r>
+      <t>'wasabi'.padRight(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //"wasabi "
+'wasabi'.padRight(8, '-') //"wasabi--"</t>
+    </r>
+  </si>
+  <si>
+    <t>remove(f)</t>
+  </si>
+  <si>
+    <r>
+      <t>schfifty five'.remove('</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>') //"schifty five"
+'schfifty five'.remove(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/[a-f]/g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) //"shity iv"
+</t>
+    </r>
+  </si>
+  <si>
+    <t>removeAll(f)</t>
+  </si>
+  <si>
+    <t>Removes the first occurrence of f in the string. 
+f can be a either case-sensitive string or a regex. In either case only the first match will be removed. 
+To remove multiple occurrences, use removeAll.</t>
+  </si>
+  <si>
+    <t>Removes any occurences of f in the string. 
+f can be either a case-sensitive string or a regex. In either case all matches will be removed.
+To remove only a single occurence, use remove.</t>
+  </si>
+  <si>
+    <t>schfifty five'.removeAll('f') //"schity ive"
+'schfifty five'.removeAll(/[a-f]/) //"shity iv"</t>
+  </si>
+  <si>
+    <t>removeTags([tag] = 'all',[replace])</t>
+  </si>
+  <si>
+    <t>modify String - HTML</t>
+  </si>
+  <si>
+    <t>Removes HTML tags and their contents from the string. tag may be an array of tags or 'all', in which case all tags will be removed. replace will replace what was removed, and may be a string or a function of type replaceFn to handle replacements. If this function returns a string, then it will be used for the replacement. If it returns undefined, the tags will be removed normally.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;p&gt;just &lt;b&gt;some&lt;/b&gt; text&lt;/p&gt;'.removeTags() </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//""</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+'&lt;p&gt;just &lt;b&gt;some&lt;/b&gt; text&lt;/p&gt;'.removeTags('b') </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//"&lt;p&gt;just text&lt;/p&gt;"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+'&lt;p&gt;hi!&lt;/p&gt;'.removeTags('p', function(all, content) {
+  return 'bye!';
+}); </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//"bye!"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">
+tag - The tag name.
+inner - The tag content.
+attr - The attributes on the tag, if any, as a string.
+outer - The entire matched tag string.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+line - The current line.
+i - The current index.
+arr - An array of all lines.</t>
+  </si>
+  <si>
+    <t>repeat([num] = 0)</t>
+  </si>
+  <si>
+    <t>generate String</t>
+  </si>
+  <si>
+    <t>Returns the string repeated num times. This method is provided as a polyfill.</t>
+  </si>
+  <si>
+    <r>
+      <t>'jumpy'.repeat(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //"jumpyjumpy"
+'a'.repeat(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //"aaaaa"
+'a'.repeat(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //""</t>
+    </r>
+  </si>
+  <si>
+    <t>replaceAll(f,[str1],[str2],[...)</t>
+  </si>
+  <si>
+    <t>Replaces all occurences of f with arguments passed. 
+This method is intended to be a quick way to perform multiple string replacements quickly when the replacement token differs depending on position. f can be either a case-sensitive string or a regex. In either case all matches will be replaced.</t>
+  </si>
+  <si>
+    <r>
+      <t>'-x -y -z'.replaceAll(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>', 1, 2, 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) //"1x 2y 3z"
+'one and two'.replaceAll(/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>one|two</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/, '1st', '2nd') //"1st and 2nd"</t>
+    </r>
+  </si>
+  <si>
+    <t>reverse()</t>
+  </si>
+  <si>
+    <t>Reverses the string.</t>
+  </si>
+  <si>
+    <t>jumpy'.reverse()
+'lucky charms'.reverse()</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">calc number or generate </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String</t>
     </r>
   </si>
 </sst>
@@ -11170,7 +13279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -11239,6 +13348,15 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11255,6 +13373,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>43061</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4165358</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>2061882</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0F682B4-511B-4110-B75A-BF4E8E0B37EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5977696" y="14065624"/>
+          <a:ext cx="4122297" cy="2017058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12654,8 +14821,8 @@
   </sheetPr>
   <dimension ref="A2:W130"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13544,7 +15711,7 @@
       <c r="B74" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C74" s="14" t="s">
+      <c r="C74" s="24" t="s">
         <v>150</v>
       </c>
       <c r="D74" s="14" t="s">
@@ -13624,7 +15791,7 @@
         <v>123</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>206</v>
+        <v>826</v>
       </c>
       <c r="C80" s="14" t="s">
         <v>125</v>
@@ -13641,7 +15808,7 @@
         <v>127</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>206</v>
+        <v>826</v>
       </c>
       <c r="C81" s="14" t="s">
         <v>129</v>
@@ -13907,7 +16074,7 @@
   </sheetPr>
   <dimension ref="A2:W152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -16703,8 +18870,8 @@
   </sheetPr>
   <dimension ref="A2:AB100"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18646,4 +20813,560 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D9C033-30BC-4D88-9149-0AED138B4921}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:V48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="61.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="71.21875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.21875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="43.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="55.109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="67.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="64.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.77734375" style="7" customWidth="1"/>
+    <col min="12" max="12" width="39.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="48.88671875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="72.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="43.88671875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="7.77734375" style="7" customWidth="1"/>
+    <col min="17" max="17" width="56.77734375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="46.77734375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="62.88671875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="49.21875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="8.77734375" style="8"/>
+    <col min="22" max="22" width="67.77734375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="68.33203125" style="1" customWidth="1"/>
+    <col min="24" max="25" width="59.33203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="59.6640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="99.44140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="41.21875" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.77734375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="15"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="15"/>
+      <c r="B5" s="20"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="B6" s="21"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="21"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="21"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+      <c r="B9" s="20"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+      <c r="B10" s="20"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="21"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="20"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="V16" s="5"/>
+    </row>
+    <row r="19" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>724</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>730</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>746</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>729</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>728</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>734</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>738</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>742</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>750</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>753</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>758</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>761</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>765</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>763</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>768</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>772</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>775</v>
+      </c>
+      <c r="E33" s="24"/>
+    </row>
+    <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>777</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>782</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>784</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>785</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>790</v>
+      </c>
+      <c r="D38" s="24" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="D39" s="24" t="s">
+        <v>791</v>
+      </c>
+      <c r="E39" s="24" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>797</v>
+      </c>
+      <c r="D40" s="24" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>800</v>
+      </c>
+      <c r="D41" s="24" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>803</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>805</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>809</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>813</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>812</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>819</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>822</v>
+      </c>
+      <c r="D47" s="24" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>825</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>824</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>